<commit_message>
updated with work from 2/7
</commit_message>
<xml_diff>
--- a/data/swerve_tuning.xlsx
+++ b/data/swerve_tuning.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\butch\robottools\robots\swimmy2023\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE38C791-828C-4FDF-945E-8D312883DDA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3238A64-27D1-4D3F-8C23-FE9B4E0340D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{63ED495D-4CE5-48FC-B482-A94B23E9B863}"/>
   </bookViews>
@@ -276,19 +276,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.36859999999999998</c:v>
+                  <c:v>0.35549999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.34</c:v>
+                  <c:v>1.3420000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2440000000000002</c:v>
+                  <c:v>2.2370000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.1429999999999998</c:v>
+                  <c:v>3.1459999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.9729999999999999</c:v>
+                  <c:v>4.0549999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -437,7 +437,7 @@
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="25400">
           <a:noFill/>
         </a:ln>
         <a:effectLst/>
@@ -649,19 +649,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.378</c:v>
+                  <c:v>0.3604</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.339</c:v>
+                  <c:v>1.335</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.238</c:v>
+                  <c:v>2.2654000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.1579999999999999</c:v>
+                  <c:v>3.1760000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0250000000000004</c:v>
+                  <c:v>4.0430000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1022,19 +1022,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.36559999999999998</c:v>
+                  <c:v>0.35580000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2949999999999999</c:v>
+                  <c:v>1.3420000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.1589999999999998</c:v>
+                  <c:v>2.2610000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0489999999999999</c:v>
+                  <c:v>3.1720000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.86</c:v>
+                  <c:v>4.0549999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1395,19 +1395,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.36870000000000003</c:v>
+                  <c:v>0.3629</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.333</c:v>
+                  <c:v>1.335</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2309999999999999</c:v>
+                  <c:v>2.2589999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.1440000000000001</c:v>
+                  <c:v>3.1669999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0010000000000003</c:v>
+                  <c:v>4.0439999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4268,7 +4268,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4276,10 +4276,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E5122D8-8CBB-4787-B834-3424F771011E}">
-  <dimension ref="B2:F12"/>
+  <dimension ref="B2:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4306,16 +4306,16 @@
         <v>0.1</v>
       </c>
       <c r="C3">
-        <v>0.36859999999999998</v>
+        <v>0.35549999999999998</v>
       </c>
       <c r="D3">
-        <v>0.378</v>
+        <v>0.3604</v>
       </c>
       <c r="E3">
-        <v>0.36559999999999998</v>
+        <v>0.35580000000000001</v>
       </c>
       <c r="F3">
-        <v>0.36870000000000003</v>
+        <v>0.3629</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.55000000000000004">
@@ -4323,16 +4323,16 @@
         <v>0.3</v>
       </c>
       <c r="C4">
-        <v>1.34</v>
+        <v>1.3420000000000001</v>
       </c>
       <c r="D4">
-        <v>1.339</v>
+        <v>1.335</v>
       </c>
       <c r="E4">
-        <v>1.2949999999999999</v>
+        <v>1.3420000000000001</v>
       </c>
       <c r="F4">
-        <v>1.333</v>
+        <v>1.335</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.55000000000000004">
@@ -4340,16 +4340,16 @@
         <v>0.5</v>
       </c>
       <c r="C5">
-        <v>2.2440000000000002</v>
+        <v>2.2370000000000001</v>
       </c>
       <c r="D5">
-        <v>2.238</v>
+        <v>2.2654000000000001</v>
       </c>
       <c r="E5">
-        <v>2.1589999999999998</v>
+        <v>2.2610000000000001</v>
       </c>
       <c r="F5">
-        <v>2.2309999999999999</v>
+        <v>2.2589999999999999</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.55000000000000004">
@@ -4357,16 +4357,16 @@
         <v>0.7</v>
       </c>
       <c r="C6">
-        <v>3.1429999999999998</v>
+        <v>3.1459999999999999</v>
       </c>
       <c r="D6">
-        <v>3.1579999999999999</v>
+        <v>3.1760000000000002</v>
       </c>
       <c r="E6">
-        <v>3.0489999999999999</v>
+        <v>3.1720000000000002</v>
       </c>
       <c r="F6">
-        <v>3.1440000000000001</v>
+        <v>3.1669999999999998</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.55000000000000004">
@@ -4374,16 +4374,16 @@
         <v>0.9</v>
       </c>
       <c r="C7">
-        <v>3.9729999999999999</v>
+        <v>4.0549999999999997</v>
       </c>
       <c r="D7">
-        <v>4.0250000000000004</v>
+        <v>4.0430000000000001</v>
       </c>
       <c r="E7">
-        <v>3.86</v>
+        <v>4.0549999999999997</v>
       </c>
       <c r="F7">
-        <v>4.0010000000000003</v>
+        <v>4.0439999999999996</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.55000000000000004">
@@ -4391,16 +4391,16 @@
         <v>5</v>
       </c>
       <c r="C9">
-        <v>4.4465000000000003</v>
+        <v>4.4898999999999996</v>
       </c>
       <c r="D9">
-        <v>4.4798</v>
+        <v>4.5037000000000003</v>
       </c>
       <c r="E9">
-        <v>4.3108000000000004</v>
+        <v>4.5082000000000004</v>
       </c>
       <c r="F9">
-        <v>4.4569999999999999</v>
+        <v>4.4987000000000004</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.55000000000000004">
@@ -4426,19 +4426,89 @@
       </c>
       <c r="C12">
         <f>1/C9</f>
-        <v>0.22489598560665691</v>
+        <v>0.22272210962382238</v>
       </c>
       <c r="D12">
         <f>1/D9</f>
-        <v>0.22322425108263763</v>
+        <v>0.22203965628261207</v>
       </c>
       <c r="E12">
         <f>1/E9</f>
-        <v>0.23197550338684234</v>
+        <v>0.22181802049598506</v>
       </c>
       <c r="F12">
         <f>1/F9</f>
-        <v>0.22436616558223021</v>
+        <v>0.22228643830439904</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18">
+        <v>0.36859999999999998</v>
+      </c>
+      <c r="C18">
+        <v>0.378</v>
+      </c>
+      <c r="D18">
+        <v>0.36559999999999998</v>
+      </c>
+      <c r="E18">
+        <v>0.36870000000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19">
+        <v>1.34</v>
+      </c>
+      <c r="C19">
+        <v>1.339</v>
+      </c>
+      <c r="D19">
+        <v>1.2949999999999999</v>
+      </c>
+      <c r="E19">
+        <v>1.333</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B20">
+        <v>2.2440000000000002</v>
+      </c>
+      <c r="C20">
+        <v>2.238</v>
+      </c>
+      <c r="D20">
+        <v>2.1589999999999998</v>
+      </c>
+      <c r="E20">
+        <v>2.2309999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21">
+        <v>3.1429999999999998</v>
+      </c>
+      <c r="C21">
+        <v>3.1579999999999999</v>
+      </c>
+      <c r="D21">
+        <v>3.0489999999999999</v>
+      </c>
+      <c r="E21">
+        <v>3.1440000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22">
+        <v>3.9729999999999999</v>
+      </c>
+      <c r="C22">
+        <v>4.0250000000000004</v>
+      </c>
+      <c r="D22">
+        <v>3.86</v>
+      </c>
+      <c r="E22">
+        <v>4.0010000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>